<commit_message>
adding housekeeping RTD commands
</commit_message>
<xml_diff>
--- a/commands/housekeeping/housekeeping_command_deck.xlsx
+++ b/commands/housekeeping/housekeeping_command_deck.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/housekeeping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E594456F-4B9F-C244-A244-8721539DD697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27F6138-2519-EC40-9F51-035B571172C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="114">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -325,6 +325,57 @@
   </si>
   <si>
     <t>0x0e</t>
+  </si>
+  <si>
+    <t>set_temp1_init</t>
+  </si>
+  <si>
+    <t>set_temp2_init</t>
+  </si>
+  <si>
+    <t>start_temp1_convert</t>
+  </si>
+  <si>
+    <t>start_temp2_convert</t>
+  </si>
+  <si>
+    <t>read_temp1_all</t>
+  </si>
+  <si>
+    <t>read_temp2_all</t>
+  </si>
+  <si>
+    <t>0x24</t>
+  </si>
+  <si>
+    <t>temps</t>
+  </si>
+  <si>
+    <t>0xff</t>
+  </si>
+  <si>
+    <t>0xf2</t>
+  </si>
+  <si>
+    <t>start initializing temp sensor 1</t>
+  </si>
+  <si>
+    <t>start initializing temp sensor 2</t>
+  </si>
+  <si>
+    <t>start temp sensor 1 conversion</t>
+  </si>
+  <si>
+    <t>start temp sensor 2 conversion</t>
+  </si>
+  <si>
+    <t>get all RTD measurements from temp sensor 1</t>
+  </si>
+  <si>
+    <t>get all RTD measurements from temp sensor 2</t>
+  </si>
+  <si>
+    <t>0xf0</t>
   </si>
 </sst>
 </file>
@@ -336,7 +387,7 @@
     <numFmt numFmtId="165" formatCode="00\ 0000\ 00"/>
     <numFmt numFmtId="166" formatCode="0000\ ####"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -383,6 +434,13 @@
       <name val="Courier New"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -428,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -482,6 +540,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,13 +865,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F008E-2DBD-E446-BC2F-AA0D9FF4122A}">
-  <dimension ref="A1:AC38"/>
+  <dimension ref="A1:AC44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y5" sqref="Y5"/>
+      <selection pane="bottomRight" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -970,7 +1039,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f t="shared" ref="E3:E6" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
+        <f t="shared" ref="E3:E8" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
         <v>0x80</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1227,8 +1296,8 @@
       </c>
     </row>
     <row r="6" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>23</v>
+      <c r="A6" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>41</v>
@@ -1237,11 +1306,11 @@
         <v>1</v>
       </c>
       <c r="D6" s="10">
-        <v>111001</v>
+        <v>100</v>
       </c>
       <c r="E6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0xB9</v>
+        <v>0x84</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>17</v>
@@ -1256,16 +1325,16 @@
         <v>17</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="L6" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="6">
         <v>0</v>
@@ -1301,10 +1370,10 @@
         <v>48</v>
       </c>
       <c r="Y6" s="22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="AA6" s="23" t="s">
         <v>29</v>
@@ -1313,59 +1382,121 @@
         <v>51</v>
       </c>
       <c r="AC6" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="24"/>
-      <c r="Z7" s="7"/>
-      <c r="AA7" s="24"/>
+    <row r="7" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="10">
+        <v>101</v>
+      </c>
+      <c r="E7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>0x85</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" s="6">
+        <v>0</v>
+      </c>
+      <c r="M7" s="6">
+        <v>1</v>
+      </c>
+      <c r="N7" s="29">
+        <v>0</v>
+      </c>
+      <c r="O7" s="29">
+        <v>0</v>
+      </c>
+      <c r="P7" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="29">
+        <v>0</v>
+      </c>
+      <c r="R7" s="29">
+        <v>0</v>
+      </c>
+      <c r="S7" s="29">
+        <v>0</v>
+      </c>
+      <c r="T7" s="29">
+        <v>0</v>
+      </c>
+      <c r="U7" s="29">
+        <v>0</v>
+      </c>
+      <c r="V7" s="29">
+        <v>0</v>
+      </c>
+      <c r="W7" s="30">
+        <v>0</v>
+      </c>
+      <c r="X7" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y7" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z7" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA7" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB7" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="8" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="10">
-        <v>0</v>
+        <v>111001</v>
       </c>
       <c r="E8" s="3" t="str">
-        <f t="shared" ref="E8:E38" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C8,7) + BIN2DEC($D8)))</f>
-        <v>0x0</v>
+        <f t="shared" si="0"/>
+        <v>0xB9</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>17</v>
@@ -1374,16 +1505,16 @@
         <v>17</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="K8" s="23" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="L8" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="6">
         <v>0</v>
@@ -1419,7 +1550,7 @@
         <v>48</v>
       </c>
       <c r="Y8" s="22" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="Z8" s="3" t="s">
         <v>29</v>
@@ -1431,102 +1562,40 @@
         <v>51</v>
       </c>
       <c r="AC8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="10">
-        <v>100000</v>
-      </c>
-      <c r="E9" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x20</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" s="6">
-        <v>0</v>
-      </c>
-      <c r="M9" s="6">
-        <v>1</v>
-      </c>
-      <c r="N9" s="6">
-        <v>0</v>
-      </c>
-      <c r="O9" s="6">
-        <v>0</v>
-      </c>
-      <c r="P9" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="6">
-        <v>0</v>
-      </c>
-      <c r="R9" s="6">
-        <v>0</v>
-      </c>
-      <c r="S9" s="6">
-        <v>0</v>
-      </c>
-      <c r="T9" s="6">
-        <v>0</v>
-      </c>
-      <c r="U9" s="6">
-        <v>0</v>
-      </c>
-      <c r="V9" s="6">
-        <v>0</v>
-      </c>
-      <c r="W9" s="16">
-        <v>0</v>
-      </c>
-      <c r="X9" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y9" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA9" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>46</v>
-      </c>
+    <row r="9" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="24"/>
     </row>
     <row r="10" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>41</v>
@@ -1535,17 +1604,17 @@
         <v>0</v>
       </c>
       <c r="D10" s="10">
-        <v>1111</v>
+        <v>0</v>
       </c>
       <c r="E10" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0xF</v>
+        <f t="shared" ref="E10:E44" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C10,7) + BIN2DEC($D10)))</f>
+        <v>0x0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>17</v>
@@ -1611,12 +1680,12 @@
         <v>51</v>
       </c>
       <c r="AC10" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>41</v>
@@ -1625,17 +1694,17 @@
         <v>0</v>
       </c>
       <c r="D11" s="10">
-        <v>101111</v>
+        <v>100000</v>
       </c>
       <c r="E11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x2F</v>
+        <v>0x20</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>17</v>
@@ -1701,12 +1770,12 @@
         <v>51</v>
       </c>
       <c r="AC11" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>41</v>
@@ -1715,17 +1784,17 @@
         <v>0</v>
       </c>
       <c r="D12" s="10">
-        <v>1110111</v>
+        <v>1111</v>
       </c>
       <c r="E12" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x77</v>
+        <v>0xF</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>17</v>
@@ -1791,12 +1860,12 @@
         <v>51</v>
       </c>
       <c r="AC12" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
-        <v>57</v>
+      <c r="A13" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>41</v>
@@ -1805,11 +1874,11 @@
         <v>0</v>
       </c>
       <c r="D13" s="10">
-        <v>1000000</v>
+        <v>101111</v>
       </c>
       <c r="E13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x40</v>
+        <v>0x2F</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>17</v>
@@ -1868,25 +1937,25 @@
       <c r="X13" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="Y13" s="3" t="s">
-        <v>81</v>
+      <c r="Y13" s="22" t="s">
+        <v>29</v>
       </c>
       <c r="Z13" s="3" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="AA13" s="23" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="AB13" t="s">
         <v>51</v>
       </c>
       <c r="AC13" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
-        <v>58</v>
+      <c r="A14" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>41</v>
@@ -1895,17 +1964,17 @@
         <v>0</v>
       </c>
       <c r="D14" s="10">
-        <v>1100000</v>
+        <v>1110111</v>
       </c>
       <c r="E14" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x60</v>
+        <v>0x77</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>17</v>
@@ -1958,11 +2027,11 @@
       <c r="X14" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="Y14" s="3" t="s">
-        <v>81</v>
+      <c r="Y14" s="22" t="s">
+        <v>29</v>
       </c>
       <c r="Z14" s="3" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="AA14" s="23" t="s">
         <v>29</v>
@@ -1976,7 +2045,7 @@
     </row>
     <row r="15" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>41</v>
@@ -1985,11 +2054,11 @@
         <v>0</v>
       </c>
       <c r="D15" s="10">
-        <v>1001111</v>
+        <v>1000000</v>
       </c>
       <c r="E15" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x4F</v>
+        <v>0x40</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>17</v>
@@ -2052,7 +2121,7 @@
         <v>81</v>
       </c>
       <c r="Z15" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="AA15" s="23" t="s">
         <v>53</v>
@@ -2061,12 +2130,12 @@
         <v>51</v>
       </c>
       <c r="AC15" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>41</v>
@@ -2075,11 +2144,11 @@
         <v>0</v>
       </c>
       <c r="D16" s="10">
-        <v>1101111</v>
+        <v>1100000</v>
       </c>
       <c r="E16" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x6F</v>
+        <v>0x60</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>17</v>
@@ -2142,7 +2211,7 @@
         <v>81</v>
       </c>
       <c r="Z16" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="AA16" s="23" t="s">
         <v>29</v>
@@ -2151,12 +2220,12 @@
         <v>51</v>
       </c>
       <c r="AC16" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>41</v>
@@ -2165,11 +2234,11 @@
         <v>0</v>
       </c>
       <c r="D17" s="10">
-        <v>1001000</v>
+        <v>1001111</v>
       </c>
       <c r="E17" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x48</v>
+        <v>0x4F</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>17</v>
@@ -2232,7 +2301,7 @@
         <v>81</v>
       </c>
       <c r="Z17" s="3" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="AA17" s="23" t="s">
         <v>53</v>
@@ -2241,12 +2310,12 @@
         <v>51</v>
       </c>
       <c r="AC17" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>41</v>
@@ -2255,11 +2324,11 @@
         <v>0</v>
       </c>
       <c r="D18" s="10">
-        <v>1101000</v>
+        <v>1101111</v>
       </c>
       <c r="E18" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x68</v>
+        <v>0x6F</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>17</v>
@@ -2322,7 +2391,7 @@
         <v>81</v>
       </c>
       <c r="Z18" s="3" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="AA18" s="23" t="s">
         <v>29</v>
@@ -2331,12 +2400,12 @@
         <v>51</v>
       </c>
       <c r="AC18" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>41</v>
@@ -2345,11 +2414,11 @@
         <v>0</v>
       </c>
       <c r="D19" s="10">
-        <v>1000001</v>
+        <v>1001000</v>
       </c>
       <c r="E19" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x41</v>
+        <v>0x48</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>17</v>
@@ -2412,7 +2481,7 @@
         <v>81</v>
       </c>
       <c r="Z19" s="3" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="AA19" s="23" t="s">
         <v>53</v>
@@ -2426,7 +2495,7 @@
     </row>
     <row r="20" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>41</v>
@@ -2435,11 +2504,11 @@
         <v>0</v>
       </c>
       <c r="D20" s="10">
-        <v>1100001</v>
+        <v>1101000</v>
       </c>
       <c r="E20" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x61</v>
+        <v>0x68</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>17</v>
@@ -2502,7 +2571,7 @@
         <v>81</v>
       </c>
       <c r="Z20" s="3" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="AA20" s="23" t="s">
         <v>29</v>
@@ -2516,7 +2585,7 @@
     </row>
     <row r="21" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>41</v>
@@ -2525,11 +2594,11 @@
         <v>0</v>
       </c>
       <c r="D21" s="10">
-        <v>1000010</v>
+        <v>1000001</v>
       </c>
       <c r="E21" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x42</v>
+        <v>0x41</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>17</v>
@@ -2592,7 +2661,7 @@
         <v>81</v>
       </c>
       <c r="Z21" s="3" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="AA21" s="23" t="s">
         <v>53</v>
@@ -2606,7 +2675,7 @@
     </row>
     <row r="22" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>41</v>
@@ -2615,11 +2684,11 @@
         <v>0</v>
       </c>
       <c r="D22" s="10">
-        <v>1100010</v>
+        <v>1100001</v>
       </c>
       <c r="E22" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x62</v>
+        <v>0x61</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>17</v>
@@ -2682,7 +2751,7 @@
         <v>81</v>
       </c>
       <c r="Z22" s="3" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="AA22" s="23" t="s">
         <v>29</v>
@@ -2696,7 +2765,7 @@
     </row>
     <row r="23" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>41</v>
@@ -2705,11 +2774,11 @@
         <v>0</v>
       </c>
       <c r="D23" s="10">
-        <v>1000011</v>
+        <v>1000010</v>
       </c>
       <c r="E23" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x43</v>
+        <v>0x42</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>17</v>
@@ -2772,7 +2841,7 @@
         <v>81</v>
       </c>
       <c r="Z23" s="3" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="AA23" s="23" t="s">
         <v>53</v>
@@ -2786,7 +2855,7 @@
     </row>
     <row r="24" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>41</v>
@@ -2795,11 +2864,11 @@
         <v>0</v>
       </c>
       <c r="D24" s="10">
-        <v>1100011</v>
+        <v>1100010</v>
       </c>
       <c r="E24" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x63</v>
+        <v>0x62</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>17</v>
@@ -2862,7 +2931,7 @@
         <v>81</v>
       </c>
       <c r="Z24" s="3" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="AA24" s="23" t="s">
         <v>29</v>
@@ -2876,7 +2945,7 @@
     </row>
     <row r="25" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>41</v>
@@ -2885,11 +2954,11 @@
         <v>0</v>
       </c>
       <c r="D25" s="10">
-        <v>1000100</v>
+        <v>1000011</v>
       </c>
       <c r="E25" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x44</v>
+        <v>0x43</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>17</v>
@@ -2952,7 +3021,7 @@
         <v>81</v>
       </c>
       <c r="Z25" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AA25" s="23" t="s">
         <v>53</v>
@@ -2966,7 +3035,7 @@
     </row>
     <row r="26" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>41</v>
@@ -2975,11 +3044,11 @@
         <v>0</v>
       </c>
       <c r="D26" s="10">
-        <v>1100100</v>
+        <v>1100011</v>
       </c>
       <c r="E26" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x64</v>
+        <v>0x63</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>17</v>
@@ -3042,7 +3111,7 @@
         <v>81</v>
       </c>
       <c r="Z26" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AA26" s="23" t="s">
         <v>29</v>
@@ -3056,7 +3125,7 @@
     </row>
     <row r="27" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>41</v>
@@ -3065,11 +3134,11 @@
         <v>0</v>
       </c>
       <c r="D27" s="10">
-        <v>1011111</v>
+        <v>1000100</v>
       </c>
       <c r="E27" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x5F</v>
+        <v>0x44</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>17</v>
@@ -3132,7 +3201,7 @@
         <v>81</v>
       </c>
       <c r="Z27" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="AA27" s="23" t="s">
         <v>53</v>
@@ -3141,12 +3210,12 @@
         <v>51</v>
       </c>
       <c r="AC27" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>41</v>
@@ -3155,11 +3224,11 @@
         <v>0</v>
       </c>
       <c r="D28" s="10">
-        <v>1111111</v>
+        <v>1100100</v>
       </c>
       <c r="E28" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x7F</v>
+        <v>0x64</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>17</v>
@@ -3222,7 +3291,7 @@
         <v>81</v>
       </c>
       <c r="Z28" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="AA28" s="23" t="s">
         <v>29</v>
@@ -3231,12 +3300,12 @@
         <v>51</v>
       </c>
       <c r="AC28" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>41</v>
@@ -3245,11 +3314,11 @@
         <v>0</v>
       </c>
       <c r="D29" s="10">
-        <v>1010001</v>
+        <v>1011111</v>
       </c>
       <c r="E29" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x51</v>
+        <v>0x5F</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>17</v>
@@ -3312,7 +3381,7 @@
         <v>81</v>
       </c>
       <c r="Z29" s="3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="AA29" s="23" t="s">
         <v>53</v>
@@ -3321,12 +3390,12 @@
         <v>51</v>
       </c>
       <c r="AC29" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>41</v>
@@ -3335,11 +3404,11 @@
         <v>0</v>
       </c>
       <c r="D30" s="10">
-        <v>1110001</v>
+        <v>1111111</v>
       </c>
       <c r="E30" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x71</v>
+        <v>0x7F</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>17</v>
@@ -3402,7 +3471,7 @@
         <v>81</v>
       </c>
       <c r="Z30" s="3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="AA30" s="23" t="s">
         <v>29</v>
@@ -3411,12 +3480,12 @@
         <v>51</v>
       </c>
       <c r="AC30" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>41</v>
@@ -3425,11 +3494,11 @@
         <v>0</v>
       </c>
       <c r="D31" s="10">
-        <v>1010010</v>
+        <v>1010001</v>
       </c>
       <c r="E31" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x52</v>
+        <v>0x51</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>17</v>
@@ -3492,7 +3561,7 @@
         <v>81</v>
       </c>
       <c r="Z31" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AA31" s="23" t="s">
         <v>53</v>
@@ -3506,7 +3575,7 @@
     </row>
     <row r="32" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>41</v>
@@ -3515,11 +3584,11 @@
         <v>0</v>
       </c>
       <c r="D32" s="10">
-        <v>1110010</v>
+        <v>1110001</v>
       </c>
       <c r="E32" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x72</v>
+        <v>0x71</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>17</v>
@@ -3582,7 +3651,7 @@
         <v>81</v>
       </c>
       <c r="Z32" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AA32" s="23" t="s">
         <v>29</v>
@@ -3596,7 +3665,7 @@
     </row>
     <row r="33" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>41</v>
@@ -3605,11 +3674,11 @@
         <v>0</v>
       </c>
       <c r="D33" s="10">
-        <v>1010100</v>
+        <v>1010010</v>
       </c>
       <c r="E33" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x54</v>
+        <v>0x52</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>17</v>
@@ -3672,7 +3741,7 @@
         <v>81</v>
       </c>
       <c r="Z33" s="3" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="AA33" s="23" t="s">
         <v>53</v>
@@ -3686,7 +3755,7 @@
     </row>
     <row r="34" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B34" s="18" t="s">
         <v>41</v>
@@ -3695,11 +3764,11 @@
         <v>0</v>
       </c>
       <c r="D34" s="10">
-        <v>1110100</v>
+        <v>1110010</v>
       </c>
       <c r="E34" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x74</v>
+        <v>0x72</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>17</v>
@@ -3762,7 +3831,7 @@
         <v>81</v>
       </c>
       <c r="Z34" s="3" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="AA34" s="23" t="s">
         <v>29</v>
@@ -3776,7 +3845,7 @@
     </row>
     <row r="35" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B35" s="18" t="s">
         <v>41</v>
@@ -3785,11 +3854,11 @@
         <v>0</v>
       </c>
       <c r="D35" s="10">
-        <v>1011000</v>
+        <v>1010100</v>
       </c>
       <c r="E35" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x58</v>
+        <v>0x54</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>17</v>
@@ -3852,7 +3921,7 @@
         <v>81</v>
       </c>
       <c r="Z35" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AA35" s="23" t="s">
         <v>53</v>
@@ -3866,7 +3935,7 @@
     </row>
     <row r="36" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>41</v>
@@ -3875,11 +3944,11 @@
         <v>0</v>
       </c>
       <c r="D36" s="10">
-        <v>1111000</v>
+        <v>1110100</v>
       </c>
       <c r="E36" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x78</v>
+        <v>0x74</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>17</v>
@@ -3942,7 +4011,7 @@
         <v>81</v>
       </c>
       <c r="Z36" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AA36" s="23" t="s">
         <v>29</v>
@@ -3956,7 +4025,7 @@
     </row>
     <row r="37" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>41</v>
@@ -3965,11 +4034,11 @@
         <v>0</v>
       </c>
       <c r="D37" s="10">
-        <v>1011100</v>
+        <v>1011000</v>
       </c>
       <c r="E37" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x5C</v>
+        <v>0x58</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>17</v>
@@ -4032,7 +4101,7 @@
         <v>81</v>
       </c>
       <c r="Z37" s="3" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="AA37" s="23" t="s">
         <v>53</v>
@@ -4046,7 +4115,7 @@
     </row>
     <row r="38" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>41</v>
@@ -4055,11 +4124,11 @@
         <v>0</v>
       </c>
       <c r="D38" s="10">
-        <v>1111100</v>
+        <v>1111000</v>
       </c>
       <c r="E38" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x7C</v>
+        <v>0x78</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>17</v>
@@ -4122,7 +4191,7 @@
         <v>81</v>
       </c>
       <c r="Z38" s="3" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="AA38" s="23" t="s">
         <v>29</v>
@@ -4132,6 +4201,546 @@
       </c>
       <c r="AC38" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0</v>
+      </c>
+      <c r="D39" s="10">
+        <v>1011100</v>
+      </c>
+      <c r="E39" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x5C</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="L39" s="6">
+        <v>0</v>
+      </c>
+      <c r="M39" s="6">
+        <v>1</v>
+      </c>
+      <c r="N39" s="6">
+        <v>0</v>
+      </c>
+      <c r="O39" s="6">
+        <v>0</v>
+      </c>
+      <c r="P39" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="6">
+        <v>0</v>
+      </c>
+      <c r="R39" s="6">
+        <v>0</v>
+      </c>
+      <c r="S39" s="6">
+        <v>0</v>
+      </c>
+      <c r="T39" s="6">
+        <v>0</v>
+      </c>
+      <c r="U39" s="6">
+        <v>0</v>
+      </c>
+      <c r="V39" s="6">
+        <v>0</v>
+      </c>
+      <c r="W39" s="16">
+        <v>0</v>
+      </c>
+      <c r="X39" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y39" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z39" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA39" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0</v>
+      </c>
+      <c r="D40" s="10">
+        <v>1111100</v>
+      </c>
+      <c r="E40" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x7C</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K40" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="L40" s="6">
+        <v>0</v>
+      </c>
+      <c r="M40" s="6">
+        <v>1</v>
+      </c>
+      <c r="N40" s="6">
+        <v>0</v>
+      </c>
+      <c r="O40" s="6">
+        <v>0</v>
+      </c>
+      <c r="P40" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="6">
+        <v>0</v>
+      </c>
+      <c r="R40" s="6">
+        <v>0</v>
+      </c>
+      <c r="S40" s="6">
+        <v>0</v>
+      </c>
+      <c r="T40" s="6">
+        <v>0</v>
+      </c>
+      <c r="U40" s="6">
+        <v>0</v>
+      </c>
+      <c r="V40" s="6">
+        <v>0</v>
+      </c>
+      <c r="W40" s="16">
+        <v>0</v>
+      </c>
+      <c r="X40" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y40" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z40" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA40" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0</v>
+      </c>
+      <c r="D41" s="10">
+        <v>110</v>
+      </c>
+      <c r="E41" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x6</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K41" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="L41" s="6">
+        <v>0</v>
+      </c>
+      <c r="M41" s="6">
+        <v>1</v>
+      </c>
+      <c r="N41" s="6">
+        <v>0</v>
+      </c>
+      <c r="O41" s="6">
+        <v>0</v>
+      </c>
+      <c r="P41" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="6">
+        <v>0</v>
+      </c>
+      <c r="R41" s="6">
+        <v>0</v>
+      </c>
+      <c r="S41" s="6">
+        <v>0</v>
+      </c>
+      <c r="T41" s="6">
+        <v>0</v>
+      </c>
+      <c r="U41" s="6">
+        <v>0</v>
+      </c>
+      <c r="V41" s="6">
+        <v>0</v>
+      </c>
+      <c r="W41" s="16">
+        <v>0</v>
+      </c>
+      <c r="X41" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y41" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z41" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA41" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC41" s="35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0</v>
+      </c>
+      <c r="D42" s="10">
+        <v>111</v>
+      </c>
+      <c r="E42" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x7</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="L42" s="6">
+        <v>0</v>
+      </c>
+      <c r="M42" s="6">
+        <v>1</v>
+      </c>
+      <c r="N42" s="6">
+        <v>0</v>
+      </c>
+      <c r="O42" s="6">
+        <v>0</v>
+      </c>
+      <c r="P42" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="6">
+        <v>0</v>
+      </c>
+      <c r="R42" s="6">
+        <v>0</v>
+      </c>
+      <c r="S42" s="6">
+        <v>0</v>
+      </c>
+      <c r="T42" s="6">
+        <v>0</v>
+      </c>
+      <c r="U42" s="6">
+        <v>0</v>
+      </c>
+      <c r="V42" s="6">
+        <v>0</v>
+      </c>
+      <c r="W42" s="16">
+        <v>0</v>
+      </c>
+      <c r="X42" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y42" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z42" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA42" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC42" s="35" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0</v>
+      </c>
+      <c r="D43" s="10">
+        <v>100</v>
+      </c>
+      <c r="E43" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x4</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K43" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="L43" s="6">
+        <v>0</v>
+      </c>
+      <c r="M43" s="6">
+        <v>1</v>
+      </c>
+      <c r="N43" s="6">
+        <v>0</v>
+      </c>
+      <c r="O43" s="6">
+        <v>0</v>
+      </c>
+      <c r="P43" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="6">
+        <v>0</v>
+      </c>
+      <c r="R43" s="6">
+        <v>0</v>
+      </c>
+      <c r="S43" s="6">
+        <v>0</v>
+      </c>
+      <c r="T43" s="6">
+        <v>0</v>
+      </c>
+      <c r="U43" s="6">
+        <v>0</v>
+      </c>
+      <c r="V43" s="6">
+        <v>0</v>
+      </c>
+      <c r="W43" s="16">
+        <v>0</v>
+      </c>
+      <c r="X43" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y43" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z43" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA43" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC43" s="35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0</v>
+      </c>
+      <c r="D44" s="10">
+        <v>101</v>
+      </c>
+      <c r="E44" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x5</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" t="s">
+        <v>17</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K44" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="L44" s="6">
+        <v>0</v>
+      </c>
+      <c r="M44" s="6">
+        <v>1</v>
+      </c>
+      <c r="N44" s="6">
+        <v>0</v>
+      </c>
+      <c r="O44" s="6">
+        <v>0</v>
+      </c>
+      <c r="P44" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="6">
+        <v>0</v>
+      </c>
+      <c r="R44" s="6">
+        <v>0</v>
+      </c>
+      <c r="S44" s="6">
+        <v>0</v>
+      </c>
+      <c r="T44" s="6">
+        <v>0</v>
+      </c>
+      <c r="U44" s="6">
+        <v>0</v>
+      </c>
+      <c r="V44" s="6">
+        <v>0</v>
+      </c>
+      <c r="W44" s="16">
+        <v>0</v>
+      </c>
+      <c r="X44" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y44" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z44" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA44" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC44" s="35" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Flight build has +Y/CMOS2 as power 0x07, and -Y/CMOS1 as power 0x08. Swapping these in Housekeeping/power commands.
</commit_message>
<xml_diff>
--- a/commands/housekeeping/housekeeping_command_deck.xlsx
+++ b/commands/housekeeping/housekeeping_command_deck.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/housekeeping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/commands/housekeeping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27F6138-2519-EC40-9F51-035B571172C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19179F12-C665-1149-AEE2-755F3DA40633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
   <sheets>
     <sheet name="all_systems" sheetId="1" r:id="rId1"/>
@@ -486,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -531,15 +531,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -550,7 +541,15 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,10 +867,10 @@
   <dimension ref="A1:AC44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D45" sqref="D45"/>
+      <selection pane="bottomRight" activeCell="Z33" sqref="Z33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -898,43 +897,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27" t="s">
+      <c r="I1" s="33"/>
+      <c r="J1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27" t="s">
+      <c r="K1" s="33"/>
+      <c r="L1" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
       <c r="X1" s="12"/>
-      <c r="Y1" s="26" t="s">
+      <c r="Y1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="28"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="34"/>
     </row>
     <row r="2" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1426,49 +1425,49 @@
       <c r="M7" s="6">
         <v>1</v>
       </c>
-      <c r="N7" s="29">
-        <v>0</v>
-      </c>
-      <c r="O7" s="29">
-        <v>0</v>
-      </c>
-      <c r="P7" s="29">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="29">
-        <v>0</v>
-      </c>
-      <c r="R7" s="29">
-        <v>0</v>
-      </c>
-      <c r="S7" s="29">
-        <v>0</v>
-      </c>
-      <c r="T7" s="29">
-        <v>0</v>
-      </c>
-      <c r="U7" s="29">
-        <v>0</v>
-      </c>
-      <c r="V7" s="29">
-        <v>0</v>
-      </c>
-      <c r="W7" s="30">
-        <v>0</v>
-      </c>
-      <c r="X7" s="31" t="s">
+      <c r="N7" s="26">
+        <v>0</v>
+      </c>
+      <c r="O7" s="26">
+        <v>0</v>
+      </c>
+      <c r="P7" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="26">
+        <v>0</v>
+      </c>
+      <c r="R7" s="26">
+        <v>0</v>
+      </c>
+      <c r="S7" s="26">
+        <v>0</v>
+      </c>
+      <c r="T7" s="26">
+        <v>0</v>
+      </c>
+      <c r="U7" s="26">
+        <v>0</v>
+      </c>
+      <c r="V7" s="26">
+        <v>0</v>
+      </c>
+      <c r="W7" s="27">
+        <v>0</v>
+      </c>
+      <c r="X7" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="Y7" s="32" t="s">
+      <c r="Y7" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="Z7" s="33" t="s">
+      <c r="Z7" s="30" t="s">
         <v>106</v>
       </c>
       <c r="AA7" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="AB7" s="34" t="s">
+      <c r="AB7" s="31" t="s">
         <v>51</v>
       </c>
       <c r="AC7" t="s">
@@ -3561,7 +3560,7 @@
         <v>81</v>
       </c>
       <c r="Z31" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AA31" s="23" t="s">
         <v>53</v>
@@ -3651,7 +3650,7 @@
         <v>81</v>
       </c>
       <c r="Z32" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AA32" s="23" t="s">
         <v>29</v>
@@ -3741,7 +3740,7 @@
         <v>81</v>
       </c>
       <c r="Z33" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AA33" s="23" t="s">
         <v>53</v>
@@ -3831,7 +3830,7 @@
         <v>81</v>
       </c>
       <c r="Z34" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AA34" s="23" t="s">
         <v>29</v>
@@ -4469,7 +4468,7 @@
       <c r="AB41" t="s">
         <v>51</v>
       </c>
-      <c r="AC41" s="35" t="s">
+      <c r="AC41" s="3" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4559,7 +4558,7 @@
       <c r="AB42" t="s">
         <v>51</v>
       </c>
-      <c r="AC42" s="35" t="s">
+      <c r="AC42" s="3" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4649,7 +4648,7 @@
       <c r="AB43" t="s">
         <v>51</v>
       </c>
-      <c r="AC43" s="35" t="s">
+      <c r="AC43" s="3" t="s">
         <v>109</v>
       </c>
     </row>
@@ -4739,7 +4738,7 @@
       <c r="AB44" t="s">
         <v>51</v>
       </c>
-      <c r="AC44" s="35" t="s">
+      <c r="AC44" s="3" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding housekeeping commands for AD7490 and introspection
</commit_message>
<xml_diff>
--- a/commands/housekeeping/housekeeping_command_deck.xlsx
+++ b/commands/housekeeping/housekeeping_command_deck.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/commands/housekeeping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/housekeeping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19179F12-C665-1149-AEE2-755F3DA40633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8F53D6-D79C-C847-96CC-A22872BF3F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="120">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -78,45 +78,18 @@
     <t>description</t>
   </si>
   <si>
-    <t>ping</t>
-  </si>
-  <si>
     <t>reply</t>
   </si>
   <si>
-    <t>pingback</t>
-  </si>
-  <si>
     <t>—</t>
   </si>
   <si>
     <t>length [B]</t>
   </si>
   <si>
-    <t>off</t>
-  </si>
-  <si>
-    <t>on</t>
-  </si>
-  <si>
-    <t>ground_off</t>
-  </si>
-  <si>
-    <t>ground_on</t>
-  </si>
-  <si>
-    <t>read_attenuator_insert</t>
-  </si>
-  <si>
     <t>CdTe select</t>
   </si>
   <si>
-    <t>set_power_output_mask</t>
-  </si>
-  <si>
-    <t>mask</t>
-  </si>
-  <si>
     <t>instruction</t>
   </si>
   <si>
@@ -132,9 +105,6 @@
     <t>applicability</t>
   </si>
   <si>
-    <t>control power output with Formatter local SPI bus</t>
-  </si>
-  <si>
     <t>CdTeDE</t>
   </si>
   <si>
@@ -162,21 +132,9 @@
     <t>0000 0000</t>
   </si>
   <si>
-    <t>test communication with system</t>
-  </si>
-  <si>
     <t>get power output on/off mask from power distribution system</t>
   </si>
   <si>
-    <t>check if attenuator ring has been inserted</t>
-  </si>
-  <si>
-    <t>turn systems off (to power distribution system)</t>
-  </si>
-  <si>
-    <t>turn systems on (to power distribution system)</t>
-  </si>
-  <si>
     <t>turn systems on or off (to power distribution system)</t>
   </si>
   <si>
@@ -186,9 +144,6 @@
     <t>outputs</t>
   </si>
   <si>
-    <t>bool</t>
-  </si>
-  <si>
     <t>todo</t>
   </si>
   <si>
@@ -204,9 +159,6 @@
     <t>write_value</t>
   </si>
   <si>
-    <t>0x4d</t>
-  </si>
-  <si>
     <t>set_power_all_off</t>
   </si>
   <si>
@@ -222,12 +174,6 @@
     <t>set_power_cdte1_off</t>
   </si>
   <si>
-    <t>set_power_cdte_all_off</t>
-  </si>
-  <si>
-    <t>set_power_cdte_all_on</t>
-  </si>
-  <si>
     <t>set_power_cdte1_on</t>
   </si>
   <si>
@@ -273,12 +219,6 @@
     <t>set_power_timepix_on</t>
   </si>
   <si>
-    <t>set_power_cmos_all_off</t>
-  </si>
-  <si>
-    <t>set_power_cmos_all_on</t>
-  </si>
-  <si>
     <t>0x03</t>
   </si>
   <si>
@@ -309,15 +249,6 @@
     <t>0x09</t>
   </si>
   <si>
-    <t>0x10</t>
-  </si>
-  <si>
-    <t>0x11</t>
-  </si>
-  <si>
-    <t>turn systems on or off (to power distribution system). NOTE: this command should be intercepted and handled by the Housekeeping board.</t>
-  </si>
-  <si>
     <t>read_power_output07_mask</t>
   </si>
   <si>
@@ -376,6 +307,93 @@
   </si>
   <si>
     <t>0xf0</t>
+  </si>
+  <si>
+    <t>set_power_health_setup</t>
+  </si>
+  <si>
+    <t>setup AD7490 power health monitor</t>
+  </si>
+  <si>
+    <t>read_power_health_all</t>
+  </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>0x20</t>
+  </si>
+  <si>
+    <t>get all power health measurements from power distribution system</t>
+  </si>
+  <si>
+    <t>set_intro_reset_errors</t>
+  </si>
+  <si>
+    <t>0xe0</t>
+  </si>
+  <si>
+    <t>set_intro_state_unlaunch</t>
+  </si>
+  <si>
+    <t>set_intro_state_await</t>
+  </si>
+  <si>
+    <t>set_intro_state_prelaunch</t>
+  </si>
+  <si>
+    <t>set_intro_state_shutter</t>
+  </si>
+  <si>
+    <t>set_intro_state_end</t>
+  </si>
+  <si>
+    <t>Formatter must handle this explicitly, should transmit 0x07e00000</t>
+  </si>
+  <si>
+    <t>Set state to waiting</t>
+  </si>
+  <si>
+    <t>Set state to prelaunch (PPS will output)</t>
+  </si>
+  <si>
+    <t>Set state to cancel PPS output</t>
+  </si>
+  <si>
+    <t>Set state to shutter open</t>
+  </si>
+  <si>
+    <t>Set state to end-of-flight</t>
+  </si>
+  <si>
+    <t>read_intro_state</t>
+  </si>
+  <si>
+    <t>read_intro_errors</t>
+  </si>
+  <si>
+    <t>read_intro_clock</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>errors</t>
+  </si>
+  <si>
+    <t>clock</t>
+  </si>
+  <si>
+    <t>0x0b</t>
+  </si>
+  <si>
+    <t>get microcontroller core clock counter (uint16_t)</t>
+  </si>
+  <si>
+    <t>get flight state value from microcontroller</t>
+  </si>
+  <si>
+    <t>get all error flags from microcontroller</t>
   </si>
 </sst>
 </file>
@@ -486,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -550,6 +568,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,10 +887,10 @@
   <dimension ref="A1:AC44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z33" sqref="Z33"/>
+      <selection pane="bottomRight" activeCell="K38" sqref="K37:K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -911,11 +931,11 @@
       </c>
       <c r="I1" s="33"/>
       <c r="J1" s="33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K1" s="33"/>
       <c r="L1" s="33" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="M1" s="33"/>
       <c r="N1" s="33"/>
@@ -930,7 +950,7 @@
       <c r="W1" s="33"/>
       <c r="X1" s="12"/>
       <c r="Y1" s="32" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="Z1" s="33"/>
       <c r="AA1" s="34"/>
@@ -940,7 +960,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
@@ -955,25 +975,25 @@
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>8</v>
@@ -982,25 +1002,25 @@
         <v>9</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="W2" s="15" t="s">
         <v>10</v>
@@ -1009,13 +1029,13 @@
         <v>11</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>12</v>
@@ -1025,39 +1045,39 @@
       </c>
     </row>
     <row r="3" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
+      <c r="A3" s="19" t="s">
+        <v>71</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" s="10">
-        <v>0</v>
+        <v>1001110</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f t="shared" ref="E3:E8" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
-        <v>0x80</v>
+        <f t="shared" ref="E3:E10" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
+        <v>0xCE</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="L3" s="6">
         <v>0</v>
@@ -1066,88 +1086,88 @@
         <v>1</v>
       </c>
       <c r="N3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="6">
         <v>0</v>
       </c>
       <c r="P3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W3" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y3" s="22" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA3" s="25" t="s">
-        <v>29</v>
+        <v>73</v>
+      </c>
+      <c r="AA3" s="23" t="s">
+        <v>20</v>
       </c>
       <c r="AB3" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" s="10">
-        <v>1001110</v>
+        <v>1001111</v>
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0xCE</v>
+        <v>0xCF</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="L4" s="6">
         <v>0</v>
@@ -1186,58 +1206,58 @@
         <v>0</v>
       </c>
       <c r="X4" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y4" s="22" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="AA4" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AB4" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC4" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" s="10">
-        <v>1001111</v>
+        <v>100</v>
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0xCF</v>
+        <v>0x84</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="L5" s="6">
         <v>0</v>
@@ -1276,58 +1296,58 @@
         <v>0</v>
       </c>
       <c r="X5" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y5" s="22" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="Z5" s="3" t="s">
         <v>83</v>
       </c>
       <c r="AA5" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AB5" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC5" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="10">
         <v>101</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="10">
-        <v>100</v>
       </c>
       <c r="E6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0x84</v>
+        <v>0x85</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="L6" s="6">
         <v>0</v>
@@ -1335,89 +1355,89 @@
       <c r="M6" s="6">
         <v>1</v>
       </c>
-      <c r="N6" s="6">
-        <v>0</v>
-      </c>
-      <c r="O6" s="6">
-        <v>0</v>
-      </c>
-      <c r="P6" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="6">
-        <v>0</v>
-      </c>
-      <c r="R6" s="6">
-        <v>0</v>
-      </c>
-      <c r="S6" s="6">
-        <v>0</v>
-      </c>
-      <c r="T6" s="6">
-        <v>0</v>
-      </c>
-      <c r="U6" s="6">
-        <v>0</v>
-      </c>
-      <c r="V6" s="6">
-        <v>0</v>
-      </c>
-      <c r="W6" s="16">
-        <v>0</v>
-      </c>
-      <c r="X6" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y6" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z6" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA6" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>51</v>
+      <c r="N6" s="26">
+        <v>0</v>
+      </c>
+      <c r="O6" s="26">
+        <v>0</v>
+      </c>
+      <c r="P6" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="26">
+        <v>0</v>
+      </c>
+      <c r="R6" s="26">
+        <v>0</v>
+      </c>
+      <c r="S6" s="26">
+        <v>0</v>
+      </c>
+      <c r="T6" s="26">
+        <v>0</v>
+      </c>
+      <c r="U6" s="26">
+        <v>0</v>
+      </c>
+      <c r="V6" s="26">
+        <v>0</v>
+      </c>
+      <c r="W6" s="27">
+        <v>0</v>
+      </c>
+      <c r="X6" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y6" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z6" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA6" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB6" s="31" t="s">
+        <v>36</v>
       </c>
       <c r="AC6" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
       <c r="D7" s="10">
-        <v>101</v>
+        <v>100000</v>
       </c>
       <c r="E7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0x85</v>
+        <v>0xA0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="L7" s="6">
         <v>0</v>
@@ -1456,176 +1476,238 @@
         <v>0</v>
       </c>
       <c r="X7" s="28" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y7" s="29" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="Z7" s="30" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="AA7" s="25" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AB7" s="31" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC7" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>23</v>
+      <c r="A8" s="19" t="s">
+        <v>110</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
       </c>
       <c r="D8" s="10">
-        <v>111001</v>
+        <v>1110000</v>
       </c>
       <c r="E8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0xB9</v>
+        <v>0xF0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="K8" s="23" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="L8" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="6">
-        <v>0</v>
-      </c>
-      <c r="N8" s="6">
-        <v>0</v>
-      </c>
-      <c r="O8" s="6">
-        <v>0</v>
-      </c>
-      <c r="P8" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="6">
-        <v>0</v>
-      </c>
-      <c r="R8" s="6">
-        <v>0</v>
-      </c>
-      <c r="S8" s="6">
-        <v>0</v>
-      </c>
-      <c r="T8" s="6">
-        <v>0</v>
-      </c>
-      <c r="U8" s="6">
-        <v>0</v>
-      </c>
-      <c r="V8" s="6">
-        <v>0</v>
-      </c>
-      <c r="W8" s="16">
-        <v>0</v>
-      </c>
-      <c r="X8" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y8" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA8" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="N8" s="26">
+        <v>0</v>
+      </c>
+      <c r="O8" s="26">
+        <v>0</v>
+      </c>
+      <c r="P8" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="26">
+        <v>0</v>
+      </c>
+      <c r="R8" s="26">
+        <v>0</v>
+      </c>
+      <c r="S8" s="26">
+        <v>0</v>
+      </c>
+      <c r="T8" s="26">
+        <v>0</v>
+      </c>
+      <c r="U8" s="26">
+        <v>0</v>
+      </c>
+      <c r="V8" s="26">
+        <v>0</v>
+      </c>
+      <c r="W8" s="27">
+        <v>0</v>
+      </c>
+      <c r="X8" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y8" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z8" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA8" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB8" s="31" t="s">
+        <v>36</v>
       </c>
       <c r="AC8" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
-      <c r="W9" s="17"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="24"/>
-      <c r="Z9" s="7"/>
-      <c r="AA9" s="24"/>
+    <row r="9" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="10">
+        <v>1111</v>
+      </c>
+      <c r="E9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>0x8F</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="K9" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="6">
+        <v>0</v>
+      </c>
+      <c r="M9" s="6">
+        <v>1</v>
+      </c>
+      <c r="N9" s="26">
+        <v>0</v>
+      </c>
+      <c r="O9" s="26">
+        <v>0</v>
+      </c>
+      <c r="P9" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="26">
+        <v>0</v>
+      </c>
+      <c r="R9" s="26">
+        <v>0</v>
+      </c>
+      <c r="S9" s="26">
+        <v>0</v>
+      </c>
+      <c r="T9" s="26">
+        <v>0</v>
+      </c>
+      <c r="U9" s="26">
+        <v>0</v>
+      </c>
+      <c r="V9" s="26">
+        <v>0</v>
+      </c>
+      <c r="W9" s="27">
+        <v>0</v>
+      </c>
+      <c r="X9" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y9" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z9" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA9" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB9" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="10" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>19</v>
+      <c r="A10" s="19" t="s">
+        <v>112</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="10">
-        <v>0</v>
+        <v>1110</v>
       </c>
       <c r="E10" s="3" t="str">
-        <f t="shared" ref="E10:E44" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C10,7) + BIN2DEC($D10)))</f>
-        <v>0x0</v>
+        <f t="shared" si="0"/>
+        <v>0x8E</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="K10" s="23" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="L10" s="6">
         <v>0</v>
@@ -1633,179 +1715,117 @@
       <c r="M10" s="6">
         <v>1</v>
       </c>
-      <c r="N10" s="6">
-        <v>0</v>
-      </c>
-      <c r="O10" s="6">
-        <v>0</v>
-      </c>
-      <c r="P10" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>0</v>
-      </c>
-      <c r="R10" s="6">
-        <v>0</v>
-      </c>
-      <c r="S10" s="6">
-        <v>0</v>
-      </c>
-      <c r="T10" s="6">
-        <v>0</v>
-      </c>
-      <c r="U10" s="6">
-        <v>0</v>
-      </c>
-      <c r="V10" s="6">
-        <v>0</v>
-      </c>
-      <c r="W10" s="16">
-        <v>0</v>
-      </c>
-      <c r="X10" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y10" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA10" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>51</v>
+      <c r="N10" s="26">
+        <v>0</v>
+      </c>
+      <c r="O10" s="26">
+        <v>0</v>
+      </c>
+      <c r="P10" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="26">
+        <v>0</v>
+      </c>
+      <c r="R10" s="26">
+        <v>0</v>
+      </c>
+      <c r="S10" s="26">
+        <v>0</v>
+      </c>
+      <c r="T10" s="26">
+        <v>0</v>
+      </c>
+      <c r="U10" s="26">
+        <v>0</v>
+      </c>
+      <c r="V10" s="26">
+        <v>0</v>
+      </c>
+      <c r="W10" s="27">
+        <v>0</v>
+      </c>
+      <c r="X10" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y10" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z10" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA10" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB10" s="31" t="s">
+        <v>36</v>
       </c>
       <c r="AC10" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="10">
-        <v>100000</v>
-      </c>
-      <c r="E11" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x20</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="6">
-        <v>0</v>
-      </c>
-      <c r="M11" s="6">
-        <v>1</v>
-      </c>
-      <c r="N11" s="6">
-        <v>0</v>
-      </c>
-      <c r="O11" s="6">
-        <v>0</v>
-      </c>
-      <c r="P11" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="6">
-        <v>0</v>
-      </c>
-      <c r="R11" s="6">
-        <v>0</v>
-      </c>
-      <c r="S11" s="6">
-        <v>0</v>
-      </c>
-      <c r="T11" s="6">
-        <v>0</v>
-      </c>
-      <c r="U11" s="6">
-        <v>0</v>
-      </c>
-      <c r="V11" s="6">
-        <v>0</v>
-      </c>
-      <c r="W11" s="16">
-        <v>0</v>
-      </c>
-      <c r="X11" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y11" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA11" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>46</v>
-      </c>
+    <row r="11" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="24"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="24"/>
     </row>
     <row r="12" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>21</v>
+      <c r="A12" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3">
         <v>0</v>
       </c>
       <c r="D12" s="10">
-        <v>1111</v>
+        <v>1000000</v>
       </c>
       <c r="E12" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0xF</v>
+        <f t="shared" ref="E12:E44" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C12,7) + BIN2DEC($D12)))</f>
+        <v>0x40</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K12" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L12" s="6">
         <v>0</v>
@@ -1844,58 +1864,58 @@
         <v>0</v>
       </c>
       <c r="X12" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y12" s="22" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="AA12" s="23" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="AB12" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>22</v>
+      <c r="A13" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3">
         <v>0</v>
       </c>
       <c r="D13" s="10">
-        <v>101111</v>
+        <v>1100000</v>
       </c>
       <c r="E13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x2F</v>
+        <v>0x60</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K13" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L13" s="6">
         <v>0</v>
@@ -1934,58 +1954,58 @@
         <v>0</v>
       </c>
       <c r="X13" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y13" s="22" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Z13" s="3" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="AA13" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AB13" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>25</v>
+      <c r="A14" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
       </c>
       <c r="D14" s="10">
-        <v>1110111</v>
+        <v>1001000</v>
       </c>
       <c r="E14" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x77</v>
+        <v>0x48</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K14" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L14" s="6">
         <v>0</v>
@@ -2024,58 +2044,58 @@
         <v>0</v>
       </c>
       <c r="X14" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y14" s="22" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Z14" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AA14" s="23" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="AB14" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC14" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
       </c>
       <c r="D15" s="10">
-        <v>1000000</v>
+        <v>1101000</v>
       </c>
       <c r="E15" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x40</v>
+        <v>0x68</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K15" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L15" s="6">
         <v>0</v>
@@ -2114,58 +2134,58 @@
         <v>0</v>
       </c>
       <c r="X15" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y15" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z15" s="3" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="AA15" s="23" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="AB15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC15" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
       </c>
       <c r="D16" s="10">
-        <v>1100000</v>
+        <v>1000001</v>
       </c>
       <c r="E16" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x60</v>
+        <v>0x41</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K16" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L16" s="6">
         <v>0</v>
@@ -2204,58 +2224,58 @@
         <v>0</v>
       </c>
       <c r="X16" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y16" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z16" s="3" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="AA16" s="23" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="AB16" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC16" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
       </c>
       <c r="D17" s="10">
-        <v>1001111</v>
+        <v>1100001</v>
       </c>
       <c r="E17" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x4F</v>
+        <v>0x61</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L17" s="6">
         <v>0</v>
@@ -2294,58 +2314,58 @@
         <v>0</v>
       </c>
       <c r="X17" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y17" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z17" s="3" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="AA17" s="23" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="AB17" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC17" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
       </c>
       <c r="D18" s="10">
-        <v>1101111</v>
+        <v>1000010</v>
       </c>
       <c r="E18" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x6F</v>
+        <v>0x42</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L18" s="6">
         <v>0</v>
@@ -2384,58 +2404,58 @@
         <v>0</v>
       </c>
       <c r="X18" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y18" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z18" s="3" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="AA18" s="23" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="AB18" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC18" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
       </c>
       <c r="D19" s="10">
-        <v>1001000</v>
+        <v>1100010</v>
       </c>
       <c r="E19" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x48</v>
+        <v>0x62</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L19" s="6">
         <v>0</v>
@@ -2474,58 +2494,58 @@
         <v>0</v>
       </c>
       <c r="X19" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y19" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z19" s="3" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="AA19" s="23" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="AB19" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC19" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
       </c>
       <c r="D20" s="10">
-        <v>1101000</v>
+        <v>1000011</v>
       </c>
       <c r="E20" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x68</v>
+        <v>0x43</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K20" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L20" s="6">
         <v>0</v>
@@ -2564,58 +2584,58 @@
         <v>0</v>
       </c>
       <c r="X20" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y20" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z20" s="3" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="AA20" s="23" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="AB20" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC20" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
       </c>
       <c r="D21" s="10">
-        <v>1000001</v>
+        <v>1100011</v>
       </c>
       <c r="E21" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x41</v>
+        <v>0x63</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K21" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L21" s="6">
         <v>0</v>
@@ -2654,58 +2674,58 @@
         <v>0</v>
       </c>
       <c r="X21" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y21" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z21" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="AA21" s="23" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="AB21" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC21" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
       </c>
       <c r="D22" s="10">
-        <v>1100001</v>
+        <v>1000100</v>
       </c>
       <c r="E22" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x61</v>
+        <v>0x44</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K22" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L22" s="6">
         <v>0</v>
@@ -2744,58 +2764,58 @@
         <v>0</v>
       </c>
       <c r="X22" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y22" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z22" s="3" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="AA22" s="23" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="AB22" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC22" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
       </c>
       <c r="D23" s="10">
-        <v>1000010</v>
+        <v>1100100</v>
       </c>
       <c r="E23" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x42</v>
+        <v>0x64</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K23" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L23" s="6">
         <v>0</v>
@@ -2834,58 +2854,58 @@
         <v>0</v>
       </c>
       <c r="X23" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y23" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z23" s="3" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="AA23" s="23" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="AB23" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC23" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
       </c>
       <c r="D24" s="10">
-        <v>1100010</v>
+        <v>1010001</v>
       </c>
       <c r="E24" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x62</v>
+        <v>0x51</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K24" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L24" s="6">
         <v>0</v>
@@ -2924,58 +2944,58 @@
         <v>0</v>
       </c>
       <c r="X24" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y24" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z24" s="3" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="AA24" s="23" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="AB24" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC24" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
       </c>
       <c r="D25" s="10">
-        <v>1000011</v>
+        <v>1110001</v>
       </c>
       <c r="E25" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x43</v>
+        <v>0x71</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K25" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L25" s="6">
         <v>0</v>
@@ -3014,58 +3034,58 @@
         <v>0</v>
       </c>
       <c r="X25" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y25" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z25" s="3" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="AA25" s="23" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="AB25" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC25" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
       </c>
       <c r="D26" s="10">
-        <v>1100011</v>
+        <v>1010010</v>
       </c>
       <c r="E26" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x63</v>
+        <v>0x52</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K26" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L26" s="6">
         <v>0</v>
@@ -3104,58 +3124,58 @@
         <v>0</v>
       </c>
       <c r="X26" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y26" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z26" s="3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="AA26" s="23" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="AB26" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC26" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
       </c>
       <c r="D27" s="10">
-        <v>1000100</v>
+        <v>1110010</v>
       </c>
       <c r="E27" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x44</v>
+        <v>0x72</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K27" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L27" s="6">
         <v>0</v>
@@ -3194,58 +3214,58 @@
         <v>0</v>
       </c>
       <c r="X27" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y27" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z27" s="3" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="AA27" s="23" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="AB27" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC27" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
       </c>
       <c r="D28" s="10">
-        <v>1100100</v>
+        <v>1010100</v>
       </c>
       <c r="E28" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x64</v>
+        <v>0x54</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K28" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L28" s="6">
         <v>0</v>
@@ -3284,58 +3304,58 @@
         <v>0</v>
       </c>
       <c r="X28" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y28" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z28" s="3" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="AA28" s="23" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="AB28" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC28" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
       </c>
       <c r="D29" s="10">
-        <v>1011111</v>
+        <v>1110100</v>
       </c>
       <c r="E29" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x5F</v>
+        <v>0x74</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K29" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L29" s="6">
         <v>0</v>
@@ -3374,58 +3394,58 @@
         <v>0</v>
       </c>
       <c r="X29" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y29" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z29" s="3" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="AA29" s="23" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="AB29" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC29" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C30" s="3">
         <v>0</v>
       </c>
       <c r="D30" s="10">
-        <v>1111111</v>
+        <v>1011000</v>
       </c>
       <c r="E30" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x7F</v>
+        <v>0x58</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K30" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L30" s="6">
         <v>0</v>
@@ -3464,58 +3484,58 @@
         <v>0</v>
       </c>
       <c r="X30" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y30" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z30" s="3" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="AA30" s="23" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="AB30" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC30" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C31" s="3">
         <v>0</v>
       </c>
       <c r="D31" s="10">
-        <v>1010001</v>
+        <v>1111000</v>
       </c>
       <c r="E31" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x51</v>
+        <v>0x78</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G31" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K31" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L31" s="6">
         <v>0</v>
@@ -3554,58 +3574,58 @@
         <v>0</v>
       </c>
       <c r="X31" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y31" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z31" s="3" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="AA31" s="23" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="AB31" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC31" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C32" s="3">
         <v>0</v>
       </c>
       <c r="D32" s="10">
-        <v>1110001</v>
+        <v>1011100</v>
       </c>
       <c r="E32" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x71</v>
+        <v>0x5C</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G32" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K32" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L32" s="6">
         <v>0</v>
@@ -3644,58 +3664,58 @@
         <v>0</v>
       </c>
       <c r="X32" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y32" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z32" s="3" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="AA32" s="23" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="AB32" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC32" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C33" s="3">
         <v>0</v>
       </c>
       <c r="D33" s="10">
-        <v>1010010</v>
+        <v>1111100</v>
       </c>
       <c r="E33" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x52</v>
+        <v>0x7C</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G33" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K33" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L33" s="6">
         <v>0</v>
@@ -3734,58 +3754,58 @@
         <v>0</v>
       </c>
       <c r="X33" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y33" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Z33" s="3" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="AA33" s="23" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="AB33" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="AC33" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C34" s="3">
         <v>0</v>
       </c>
       <c r="D34" s="10">
-        <v>1110010</v>
+        <v>110</v>
       </c>
       <c r="E34" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x72</v>
+        <v>0x6</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K34" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L34" s="6">
         <v>0</v>
@@ -3824,58 +3844,58 @@
         <v>0</v>
       </c>
       <c r="X34" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y34" s="3" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="Z34" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AA34" s="23" t="s">
-        <v>29</v>
+        <v>82</v>
+      </c>
+      <c r="AA34" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="AB34" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC34" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="AC34" s="35" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C35" s="3">
         <v>0</v>
       </c>
       <c r="D35" s="10">
-        <v>1010100</v>
+        <v>111</v>
       </c>
       <c r="E35" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x54</v>
+        <v>0x7</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G35" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K35" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L35" s="6">
         <v>0</v>
@@ -3914,22 +3934,22 @@
         <v>0</v>
       </c>
       <c r="X35" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y35" s="3" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="Z35" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA35" s="23" t="s">
-        <v>53</v>
+        <v>82</v>
+      </c>
+      <c r="AA35" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="AB35" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC35" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="AC35" s="35" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -3937,35 +3957,35 @@
         <v>76</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C36" s="3">
         <v>0</v>
       </c>
       <c r="D36" s="10">
-        <v>1110100</v>
+        <v>100</v>
       </c>
       <c r="E36" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x74</v>
+        <v>0x4</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G36" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K36" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L36" s="6">
         <v>0</v>
@@ -4004,22 +4024,22 @@
         <v>0</v>
       </c>
       <c r="X36" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y36" s="3" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="Z36" s="3" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="AA36" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AB36" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC36" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="AC36" s="35" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -4027,35 +4047,35 @@
         <v>77</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C37" s="3">
         <v>0</v>
       </c>
       <c r="D37" s="10">
-        <v>1011000</v>
+        <v>101</v>
       </c>
       <c r="E37" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x58</v>
+        <v>0x5</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K37" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L37" s="6">
         <v>0</v>
@@ -4094,58 +4114,58 @@
         <v>0</v>
       </c>
       <c r="X37" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y37" s="3" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="Z37" s="3" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="AA37" s="23" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="AB37" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC37" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="AC37" s="35" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C38" s="3">
         <v>0</v>
       </c>
       <c r="D38" s="10">
-        <v>1111000</v>
+        <v>101000</v>
       </c>
       <c r="E38" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x78</v>
+        <v>0x28</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G38" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K38" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L38" s="6">
         <v>0</v>
@@ -4184,58 +4204,58 @@
         <v>0</v>
       </c>
       <c r="X38" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y38" s="3" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="Z38" s="3" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="AA38" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AB38" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC38" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="AC38" s="35" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C39" s="3">
         <v>0</v>
       </c>
       <c r="D39" s="10">
-        <v>1011100</v>
+        <v>10000</v>
       </c>
       <c r="E39" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x5C</v>
+        <v>0x10</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I39" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K39" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L39" s="6">
         <v>0</v>
@@ -4274,58 +4294,58 @@
         <v>0</v>
       </c>
       <c r="X39" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y39" s="3" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="Z39" s="3" t="s">
         <v>90</v>
       </c>
       <c r="AA39" s="23" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="AB39" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC39" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="AC39" s="35" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C40" s="3">
         <v>0</v>
       </c>
       <c r="D40" s="10">
-        <v>1111100</v>
+        <v>10001</v>
       </c>
       <c r="E40" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x7C</v>
+        <v>0x11</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G40" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K40" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L40" s="6">
         <v>0</v>
@@ -4364,58 +4384,58 @@
         <v>0</v>
       </c>
       <c r="X40" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y40" s="3" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="Z40" s="3" t="s">
         <v>90</v>
       </c>
       <c r="AA40" s="23" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="AB40" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC40" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="AC40" s="35" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C41" s="3">
         <v>0</v>
       </c>
       <c r="D41" s="10">
-        <v>110</v>
+        <v>10010</v>
       </c>
       <c r="E41" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x6</v>
+        <v>0x12</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G41" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I41" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K41" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L41" s="6">
         <v>0</v>
@@ -4454,58 +4474,58 @@
         <v>0</v>
       </c>
       <c r="X41" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y41" s="3" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="Z41" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AA41" s="25" t="s">
-        <v>29</v>
+        <v>90</v>
+      </c>
+      <c r="AA41" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="AB41" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC41" s="3" t="s">
-        <v>107</v>
+        <v>36</v>
+      </c>
+      <c r="AC41" s="35" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C42" s="3">
         <v>0</v>
       </c>
       <c r="D42" s="10">
-        <v>111</v>
+        <v>10011</v>
       </c>
       <c r="E42" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x7</v>
+        <v>0x13</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G42" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I42" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K42" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L42" s="6">
         <v>0</v>
@@ -4544,58 +4564,58 @@
         <v>0</v>
       </c>
       <c r="X42" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y42" s="3" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="Z42" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AA42" s="25" t="s">
-        <v>29</v>
+        <v>90</v>
+      </c>
+      <c r="AA42" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="AB42" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC42" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC42" s="35" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C43" s="3">
         <v>0</v>
       </c>
       <c r="D43" s="10">
-        <v>100</v>
+        <v>10100</v>
       </c>
       <c r="E43" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x4</v>
+        <v>0x14</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G43" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I43" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K43" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L43" s="6">
         <v>0</v>
@@ -4634,58 +4654,58 @@
         <v>0</v>
       </c>
       <c r="X43" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y43" s="3" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="Z43" s="3" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="AA43" s="23" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="AB43" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC43" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC43" s="35" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C44" s="3">
         <v>0</v>
       </c>
       <c r="D44" s="10">
-        <v>101</v>
+        <v>1110</v>
       </c>
       <c r="E44" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x5</v>
+        <v>0xE</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G44" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I44" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K44" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L44" s="6">
         <v>0</v>
@@ -4724,22 +4744,22 @@
         <v>0</v>
       </c>
       <c r="X44" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y44" s="3" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="Z44" s="3" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="AA44" s="23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AB44" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC44" s="3" t="s">
-        <v>110</v>
+        <v>36</v>
+      </c>
+      <c r="AC44" s="36" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding housekeeping > clear_formatter_logs command
</commit_message>
<xml_diff>
--- a/commands/housekeeping/housekeeping_command_deck.xlsx
+++ b/commands/housekeeping/housekeeping_command_deck.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/GSE/GSE-FOXSI-4/foxsi4-commands/commands/housekeeping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/housekeeping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8FA84C-C602-9745-ADEF-A287491BAB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45765B66-8B50-FA4F-9F33-E89D213EB4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
   <sheets>
     <sheet name="all_systems" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="139">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -442,6 +442,15 @@
   </si>
   <si>
     <t>0xff1741</t>
+  </si>
+  <si>
+    <t>clear_formatter_logs</t>
+  </si>
+  <si>
+    <t>0x7f</t>
+  </si>
+  <si>
+    <t>Formatter must handle this, delete log files in formatter and truncate system logs</t>
   </si>
 </sst>
 </file>
@@ -613,6 +622,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -622,7 +632,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -937,13 +946,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F008E-2DBD-E446-BC2F-AA0D9FF4122A}">
-  <dimension ref="A1:AF48"/>
+  <dimension ref="A1:AF49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="U3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="P26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AF3" sqref="AF3"/>
+      <selection pane="bottomRight" activeCell="AE50" sqref="AE50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -972,43 +981,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33" t="s">
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33" t="s">
+      <c r="G1" s="34"/>
+      <c r="H1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33" t="s">
+      <c r="I1" s="34"/>
+      <c r="J1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33" t="s">
+      <c r="K1" s="34"/>
+      <c r="L1" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
       <c r="X1" s="12"/>
-      <c r="Y1" s="32" t="s">
+      <c r="Y1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="34"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="35"/>
       <c r="AB1" s="2"/>
       <c r="AC1" s="2"/>
     </row>
@@ -1202,7 +1211,7 @@
       <c r="AE3" t="s">
         <v>32</v>
       </c>
-      <c r="AF3" s="35"/>
+      <c r="AF3" s="32"/>
     </row>
     <row r="4" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
@@ -1920,7 +1929,7 @@
         <v>1000000</v>
       </c>
       <c r="E12" s="3" t="str">
-        <f t="shared" ref="E12:E48" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C12,7) + BIN2DEC($D12)))</f>
+        <f t="shared" ref="E12:E49" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C12,7) + BIN2DEC($D12)))</f>
         <v>0x40</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -5456,6 +5465,102 @@
       </c>
       <c r="AE48" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" s="3">
+        <v>0</v>
+      </c>
+      <c r="D49" s="10">
+        <v>1111111</v>
+      </c>
+      <c r="E49" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x7F</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G49" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K49" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="L49" s="6">
+        <v>1</v>
+      </c>
+      <c r="M49" s="6">
+        <v>0</v>
+      </c>
+      <c r="N49" s="6">
+        <v>0</v>
+      </c>
+      <c r="O49" s="6">
+        <v>0</v>
+      </c>
+      <c r="P49" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="6">
+        <v>0</v>
+      </c>
+      <c r="R49" s="6">
+        <v>0</v>
+      </c>
+      <c r="S49" s="6">
+        <v>0</v>
+      </c>
+      <c r="T49" s="6">
+        <v>0</v>
+      </c>
+      <c r="U49" s="6">
+        <v>0</v>
+      </c>
+      <c r="V49" s="6">
+        <v>0</v>
+      </c>
+      <c r="W49" s="16">
+        <v>0</v>
+      </c>
+      <c r="X49" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y49" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z49" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA49" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB49" s="3">
+        <v>25</v>
+      </c>
+      <c r="AC49" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD49" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE49" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct housekeeping command display order
</commit_message>
<xml_diff>
--- a/commands/housekeeping/housekeeping_command_deck.xlsx
+++ b/commands/housekeeping/housekeeping_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/housekeeping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45765B66-8B50-FA4F-9F33-E89D213EB4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6105E55D-04CC-DA4A-80C0-0228545A3AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -949,10 +949,10 @@
   <dimension ref="A1:AF49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="P26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE50" sqref="AE50"/>
+      <selection pane="bottomRight" activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1200,7 +1200,7 @@
         <v>20</v>
       </c>
       <c r="AB3" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AC3" s="3" t="s">
         <v>134</v>
@@ -1297,7 +1297,7 @@
         <v>20</v>
       </c>
       <c r="AB4" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AC4" s="3" t="s">
         <v>134</v>
@@ -1393,7 +1393,7 @@
         <v>20</v>
       </c>
       <c r="AB5" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC5" s="3" t="s">
         <v>134</v>
@@ -1489,7 +1489,7 @@
         <v>20</v>
       </c>
       <c r="AB6" s="30">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC6" s="3" t="s">
         <v>134</v>
@@ -1585,7 +1585,7 @@
         <v>20</v>
       </c>
       <c r="AB7" s="30">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AC7" s="3" t="s">
         <v>134</v>
@@ -1681,7 +1681,7 @@
         <v>20</v>
       </c>
       <c r="AB8" s="30">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC8" s="3" t="s">
         <v>134</v>
@@ -1777,7 +1777,7 @@
         <v>20</v>
       </c>
       <c r="AB9" s="30">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC9" s="3" t="s">
         <v>134</v>
@@ -1873,7 +1873,7 @@
         <v>20</v>
       </c>
       <c r="AB10" s="30">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AC10" s="3" t="s">
         <v>134</v>
@@ -1999,7 +1999,7 @@
         <v>38</v>
       </c>
       <c r="AB12" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AC12" s="3" t="s">
         <v>134</v>
@@ -2095,7 +2095,7 @@
         <v>20</v>
       </c>
       <c r="AB13" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AC13" s="3" t="s">
         <v>134</v>
@@ -4111,7 +4111,7 @@
         <v>20</v>
       </c>
       <c r="AB34" s="30">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AC34" s="3" t="s">
         <v>134</v>
@@ -4207,7 +4207,7 @@
         <v>20</v>
       </c>
       <c r="AB35" s="30">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC35" s="3" t="s">
         <v>134</v>
@@ -4303,7 +4303,7 @@
         <v>20</v>
       </c>
       <c r="AB36" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AC36" s="3" t="s">
         <v>134</v>
@@ -4399,7 +4399,7 @@
         <v>20</v>
       </c>
       <c r="AB37" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AC37" s="3" t="s">
         <v>134</v>
@@ -4495,7 +4495,7 @@
         <v>20</v>
       </c>
       <c r="AB38" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC38" s="3" t="s">
         <v>134</v>
@@ -4591,7 +4591,7 @@
         <v>20</v>
       </c>
       <c r="AB39" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC39" s="3" t="s">
         <v>134</v>
@@ -4687,7 +4687,7 @@
         <v>38</v>
       </c>
       <c r="AB40" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AC40" s="3" t="s">
         <v>134</v>
@@ -4783,7 +4783,7 @@
         <v>37</v>
       </c>
       <c r="AB41" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AC41" s="3" t="s">
         <v>134</v>
@@ -4879,7 +4879,7 @@
         <v>61</v>
       </c>
       <c r="AB42" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AC42" s="3" t="s">
         <v>134</v>
@@ -4975,7 +4975,7 @@
         <v>39</v>
       </c>
       <c r="AB43" s="3">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC43" s="3" t="s">
         <v>134</v>
@@ -5071,7 +5071,7 @@
         <v>20</v>
       </c>
       <c r="AB44" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AC44" s="3" t="s">
         <v>134</v>

</xml_diff>

<commit_message>
changing housekeeping > clear_formatter_logs raw command value
</commit_message>
<xml_diff>
--- a/commands/housekeeping/housekeeping_command_deck.xlsx
+++ b/commands/housekeeping/housekeeping_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/housekeeping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6105E55D-04CC-DA4A-80C0-0228545A3AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C2728D-3087-5F40-930E-1F1D692F6D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -447,10 +447,10 @@
     <t>clear_formatter_logs</t>
   </si>
   <si>
-    <t>0x7f</t>
-  </si>
-  <si>
     <t>Formatter must handle this, delete log files in formatter and truncate system logs</t>
+  </si>
+  <si>
+    <t>0x3f</t>
   </si>
 </sst>
 </file>
@@ -949,10 +949,10 @@
   <dimension ref="A1:AF49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AB14" sqref="AB14"/>
+      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -5478,11 +5478,11 @@
         <v>0</v>
       </c>
       <c r="D49" s="10">
-        <v>1111111</v>
+        <v>111111</v>
       </c>
       <c r="E49" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x7F</v>
+        <v>0x3F</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>15</v>
@@ -5542,13 +5542,13 @@
         <v>34</v>
       </c>
       <c r="Y49" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="Z49" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AA49" s="23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AB49" s="3">
         <v>25</v>
@@ -5560,7 +5560,7 @@
         <v>36</v>
       </c>
       <c r="AE49" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
switching housekeeping Ethernet interface to UDP
</commit_message>
<xml_diff>
--- a/commands/housekeeping/housekeeping_command_deck.xlsx
+++ b/commands/housekeeping/housekeeping_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/housekeeping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C2728D-3087-5F40-930E-1F1D692F6D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E76D91-8923-B344-8E8A-30D8E763CF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -348,9 +348,6 @@
     <t>set_intro_state_end</t>
   </si>
   <si>
-    <t>Formatter must handle this explicitly, should transmit 0x07e00000</t>
-  </si>
-  <si>
     <t>Set state to waiting</t>
   </si>
   <si>
@@ -451,6 +448,9 @@
   </si>
   <si>
     <t>0x3f</t>
+  </si>
+  <si>
+    <t>Formatter must handle this explicitly, should transmit 0x07e00</t>
   </si>
 </sst>
 </file>
@@ -949,10 +949,10 @@
   <dimension ref="A1:AF49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="Q27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
+      <selection pane="bottomRight" activeCell="AE45" sqref="AE45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1104,10 +1104,10 @@
         <v>40</v>
       </c>
       <c r="AB2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>12</v>
@@ -1203,7 +1203,7 @@
         <v>37</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD3" t="s">
         <v>36</v>
@@ -1300,7 +1300,7 @@
         <v>38</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD4" t="s">
         <v>36</v>
@@ -1396,7 +1396,7 @@
         <v>39</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD5" t="s">
         <v>36</v>
@@ -1492,7 +1492,7 @@
         <v>40</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD6" s="31" t="s">
         <v>36</v>
@@ -1588,7 +1588,7 @@
         <v>41</v>
       </c>
       <c r="AC7" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD7" s="31" t="s">
         <v>36</v>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="8" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>31</v>
@@ -1627,7 +1627,7 @@
         <v>15</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K8" s="23" t="s">
         <v>37</v>
@@ -1684,18 +1684,18 @@
         <v>42</v>
       </c>
       <c r="AC8" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD8" s="31" t="s">
         <v>36</v>
       </c>
       <c r="AE8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>31</v>
@@ -1723,7 +1723,7 @@
         <v>15</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K9" s="23" t="s">
         <v>37</v>
@@ -1780,18 +1780,18 @@
         <v>43</v>
       </c>
       <c r="AC9" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD9" s="31" t="s">
         <v>36</v>
       </c>
       <c r="AE9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>31</v>
@@ -1819,7 +1819,7 @@
         <v>15</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K10" s="23" t="s">
         <v>37</v>
@@ -1867,7 +1867,7 @@
         <v>66</v>
       </c>
       <c r="Z10" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AA10" s="25" t="s">
         <v>20</v>
@@ -1876,13 +1876,13 @@
         <v>44</v>
       </c>
       <c r="AC10" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD10" s="31" t="s">
         <v>36</v>
       </c>
       <c r="AE10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:32" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2002,7 +2002,7 @@
         <v>45</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD12" t="s">
         <v>36</v>
@@ -2098,7 +2098,7 @@
         <v>46</v>
       </c>
       <c r="AC13" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD13" t="s">
         <v>36</v>
@@ -2194,7 +2194,7 @@
         <v>2</v>
       </c>
       <c r="AC14" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD14" t="s">
         <v>36</v>
@@ -2290,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="AC15" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD15" t="s">
         <v>36</v>
@@ -2386,7 +2386,7 @@
         <v>4</v>
       </c>
       <c r="AC16" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AD16" t="s">
         <v>36</v>
@@ -2482,7 +2482,7 @@
         <v>3</v>
       </c>
       <c r="AC17" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD17" t="s">
         <v>36</v>
@@ -2578,7 +2578,7 @@
         <v>6</v>
       </c>
       <c r="AC18" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AD18" t="s">
         <v>36</v>
@@ -2674,7 +2674,7 @@
         <v>5</v>
       </c>
       <c r="AC19" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD19" t="s">
         <v>36</v>
@@ -2770,7 +2770,7 @@
         <v>8</v>
       </c>
       <c r="AC20" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AD20" t="s">
         <v>36</v>
@@ -2866,7 +2866,7 @@
         <v>7</v>
       </c>
       <c r="AC21" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD21" t="s">
         <v>36</v>
@@ -2962,7 +2962,7 @@
         <v>10</v>
       </c>
       <c r="AC22" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AD22" t="s">
         <v>36</v>
@@ -3058,7 +3058,7 @@
         <v>9</v>
       </c>
       <c r="AC23" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD23" t="s">
         <v>36</v>
@@ -3154,7 +3154,7 @@
         <v>12</v>
       </c>
       <c r="AC24" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AD24" t="s">
         <v>36</v>
@@ -3250,7 +3250,7 @@
         <v>11</v>
       </c>
       <c r="AC25" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD25" t="s">
         <v>36</v>
@@ -3346,7 +3346,7 @@
         <v>14</v>
       </c>
       <c r="AC26" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AD26" t="s">
         <v>36</v>
@@ -3442,7 +3442,7 @@
         <v>13</v>
       </c>
       <c r="AC27" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD27" t="s">
         <v>36</v>
@@ -3538,7 +3538,7 @@
         <v>18</v>
       </c>
       <c r="AC28" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD28" t="s">
         <v>36</v>
@@ -3634,7 +3634,7 @@
         <v>17</v>
       </c>
       <c r="AC29" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD29" t="s">
         <v>36</v>
@@ -3730,7 +3730,7 @@
         <v>16</v>
       </c>
       <c r="AC30" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD30" t="s">
         <v>36</v>
@@ -3826,7 +3826,7 @@
         <v>15</v>
       </c>
       <c r="AC31" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD31" t="s">
         <v>36</v>
@@ -3922,7 +3922,7 @@
         <v>20</v>
       </c>
       <c r="AC32" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD32" t="s">
         <v>36</v>
@@ -4018,7 +4018,7 @@
         <v>19</v>
       </c>
       <c r="AC33" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD33" t="s">
         <v>36</v>
@@ -4114,7 +4114,7 @@
         <v>26</v>
       </c>
       <c r="AC34" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD34" t="s">
         <v>36</v>
@@ -4210,7 +4210,7 @@
         <v>27</v>
       </c>
       <c r="AC35" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD35" t="s">
         <v>36</v>
@@ -4306,7 +4306,7 @@
         <v>28</v>
       </c>
       <c r="AC36" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD36" t="s">
         <v>36</v>
@@ -4402,7 +4402,7 @@
         <v>29</v>
       </c>
       <c r="AC37" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD37" t="s">
         <v>36</v>
@@ -4498,7 +4498,7 @@
         <v>30</v>
       </c>
       <c r="AC38" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD38" t="s">
         <v>36</v>
@@ -4594,13 +4594,13 @@
         <v>31</v>
       </c>
       <c r="AC39" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD39" t="s">
         <v>36</v>
       </c>
       <c r="AE39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:31" ht="16" x14ac:dyDescent="0.2">
@@ -4690,13 +4690,13 @@
         <v>32</v>
       </c>
       <c r="AC40" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD40" t="s">
         <v>36</v>
       </c>
       <c r="AE40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:31" ht="16" x14ac:dyDescent="0.2">
@@ -4786,13 +4786,13 @@
         <v>33</v>
       </c>
       <c r="AC41" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD41" t="s">
         <v>36</v>
       </c>
       <c r="AE41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:31" ht="16" x14ac:dyDescent="0.2">
@@ -4882,13 +4882,13 @@
         <v>34</v>
       </c>
       <c r="AC42" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD42" t="s">
         <v>36</v>
       </c>
       <c r="AE42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:31" ht="16" x14ac:dyDescent="0.2">
@@ -4978,13 +4978,13 @@
         <v>35</v>
       </c>
       <c r="AC43" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD43" t="s">
         <v>36</v>
       </c>
       <c r="AE43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:31" ht="16" x14ac:dyDescent="0.2">
@@ -5074,18 +5074,18 @@
         <v>36</v>
       </c>
       <c r="AC44" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD44" t="s">
         <v>36</v>
       </c>
       <c r="AE44" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B45" s="18" t="s">
         <v>31</v>
@@ -5158,10 +5158,10 @@
         <v>34</v>
       </c>
       <c r="Y45" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Z45" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AA45" s="23" t="s">
         <v>20</v>
@@ -5170,18 +5170,18 @@
         <v>21</v>
       </c>
       <c r="AC45" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD45" t="s">
         <v>36</v>
       </c>
       <c r="AE45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B46" s="18" t="s">
         <v>31</v>
@@ -5254,10 +5254,10 @@
         <v>34</v>
       </c>
       <c r="Y46" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Z46" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AA46" s="23" t="s">
         <v>20</v>
@@ -5266,18 +5266,18 @@
         <v>22</v>
       </c>
       <c r="AC46" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD46" t="s">
         <v>36</v>
       </c>
       <c r="AE46" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B47" s="18" t="s">
         <v>31</v>
@@ -5350,10 +5350,10 @@
         <v>34</v>
       </c>
       <c r="Y47" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Z47" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AA47" s="23" t="s">
         <v>20</v>
@@ -5362,18 +5362,18 @@
         <v>23</v>
       </c>
       <c r="AC47" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD47" t="s">
         <v>36</v>
       </c>
       <c r="AE47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B48" s="18" t="s">
         <v>31</v>
@@ -5446,10 +5446,10 @@
         <v>34</v>
       </c>
       <c r="Y48" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Z48" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA48" s="23" t="s">
         <v>20</v>
@@ -5458,18 +5458,18 @@
         <v>24</v>
       </c>
       <c r="AC48" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD48" t="s">
         <v>36</v>
       </c>
       <c r="AE48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B49" s="18" t="s">
         <v>31</v>
@@ -5542,25 +5542,25 @@
         <v>34</v>
       </c>
       <c r="Y49" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z49" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AA49" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AB49" s="3">
         <v>25</v>
       </c>
       <c r="AC49" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AD49" t="s">
         <v>36</v>
       </c>
       <c r="AE49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renaming cdte2 to cdte5 in housekeeping power commands
</commit_message>
<xml_diff>
--- a/commands/housekeeping/housekeeping_command_deck.xlsx
+++ b/commands/housekeeping/housekeeping_command_deck.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/housekeeping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E76D91-8923-B344-8E8A-30D8E763CF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38535B29-FB00-8E4A-93C7-9B5ED76BA88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -177,12 +177,6 @@
     <t>set_power_cdte1_on</t>
   </si>
   <si>
-    <t>set_power_cdte2_off</t>
-  </si>
-  <si>
-    <t>set_power_cdte2_on</t>
-  </si>
-  <si>
     <t>set_power_cdte3_off</t>
   </si>
   <si>
@@ -451,6 +445,12 @@
   </si>
   <si>
     <t>Formatter must handle this explicitly, should transmit 0x07e00</t>
+  </si>
+  <si>
+    <t>set_power_cdte5_off</t>
+  </si>
+  <si>
+    <t>set_power_cdte5_on</t>
   </si>
 </sst>
 </file>
@@ -949,10 +949,10 @@
   <dimension ref="A1:AF49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="Q27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="Q8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE45" sqref="AE45"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1104,10 +1104,10 @@
         <v>40</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>12</v>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>31</v>
@@ -1191,10 +1191,10 @@
         <v>34</v>
       </c>
       <c r="Y3" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AA3" s="23" t="s">
         <v>20</v>
@@ -1203,7 +1203,7 @@
         <v>37</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD3" t="s">
         <v>36</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="4" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>31</v>
@@ -1288,10 +1288,10 @@
         <v>34</v>
       </c>
       <c r="Y4" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z4" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="AA4" s="23" t="s">
         <v>20</v>
@@ -1300,7 +1300,7 @@
         <v>38</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD4" t="s">
         <v>36</v>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="5" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>31</v>
@@ -1339,10 +1339,10 @@
         <v>15</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L5" s="6">
         <v>0</v>
@@ -1387,7 +1387,7 @@
         <v>38</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AA5" s="23" t="s">
         <v>20</v>
@@ -1396,18 +1396,18 @@
         <v>39</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD5" t="s">
         <v>36</v>
       </c>
       <c r="AE5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>31</v>
@@ -1435,10 +1435,10 @@
         <v>15</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L6" s="6">
         <v>0</v>
@@ -1483,7 +1483,7 @@
         <v>37</v>
       </c>
       <c r="Z6" s="30" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AA6" s="25" t="s">
         <v>20</v>
@@ -1492,18 +1492,18 @@
         <v>40</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD6" s="31" t="s">
         <v>36</v>
       </c>
       <c r="AE6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>31</v>
@@ -1531,10 +1531,10 @@
         <v>15</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L7" s="6">
         <v>0</v>
@@ -1579,7 +1579,7 @@
         <v>39</v>
       </c>
       <c r="Z7" s="30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AA7" s="25" t="s">
         <v>20</v>
@@ -1588,18 +1588,18 @@
         <v>41</v>
       </c>
       <c r="AC7" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD7" s="31" t="s">
         <v>36</v>
       </c>
       <c r="AE7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>31</v>
@@ -1627,7 +1627,7 @@
         <v>15</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K8" s="23" t="s">
         <v>37</v>
@@ -1672,10 +1672,10 @@
         <v>34</v>
       </c>
       <c r="Y8" s="29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Z8" s="30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AA8" s="25" t="s">
         <v>20</v>
@@ -1684,18 +1684,18 @@
         <v>42</v>
       </c>
       <c r="AC8" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD8" s="31" t="s">
         <v>36</v>
       </c>
       <c r="AE8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>31</v>
@@ -1723,7 +1723,7 @@
         <v>15</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K9" s="23" t="s">
         <v>37</v>
@@ -1768,10 +1768,10 @@
         <v>34</v>
       </c>
       <c r="Y9" s="29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Z9" s="30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AA9" s="25" t="s">
         <v>20</v>
@@ -1780,18 +1780,18 @@
         <v>43</v>
       </c>
       <c r="AC9" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD9" s="31" t="s">
         <v>36</v>
       </c>
       <c r="AE9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>31</v>
@@ -1819,7 +1819,7 @@
         <v>15</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K10" s="23" t="s">
         <v>37</v>
@@ -1864,10 +1864,10 @@
         <v>34</v>
       </c>
       <c r="Y10" s="29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Z10" s="30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AA10" s="25" t="s">
         <v>20</v>
@@ -1876,13 +1876,13 @@
         <v>44</v>
       </c>
       <c r="AC10" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD10" s="31" t="s">
         <v>36</v>
       </c>
       <c r="AE10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:32" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1990,10 +1990,10 @@
         <v>34</v>
       </c>
       <c r="Y12" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AA12" s="23" t="s">
         <v>38</v>
@@ -2002,7 +2002,7 @@
         <v>45</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD12" t="s">
         <v>36</v>
@@ -2086,10 +2086,10 @@
         <v>34</v>
       </c>
       <c r="Y13" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z13" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AA13" s="23" t="s">
         <v>20</v>
@@ -2098,7 +2098,7 @@
         <v>46</v>
       </c>
       <c r="AC13" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD13" t="s">
         <v>36</v>
@@ -2182,7 +2182,7 @@
         <v>34</v>
       </c>
       <c r="Y14" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z14" s="3" t="s">
         <v>20</v>
@@ -2194,7 +2194,7 @@
         <v>2</v>
       </c>
       <c r="AC14" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD14" t="s">
         <v>36</v>
@@ -2278,7 +2278,7 @@
         <v>34</v>
       </c>
       <c r="Y15" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z15" s="3" t="s">
         <v>20</v>
@@ -2290,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="AC15" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD15" t="s">
         <v>36</v>
@@ -2374,10 +2374,10 @@
         <v>34</v>
       </c>
       <c r="Y16" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z16" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AA16" s="23" t="s">
         <v>38</v>
@@ -2386,7 +2386,7 @@
         <v>4</v>
       </c>
       <c r="AC16" s="30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AD16" t="s">
         <v>36</v>
@@ -2470,10 +2470,10 @@
         <v>34</v>
       </c>
       <c r="Y17" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z17" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AA17" s="23" t="s">
         <v>20</v>
@@ -2482,7 +2482,7 @@
         <v>3</v>
       </c>
       <c r="AC17" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD17" t="s">
         <v>36</v>
@@ -2493,7 +2493,7 @@
     </row>
     <row r="18" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>47</v>
+        <v>137</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>31</v>
@@ -2566,7 +2566,7 @@
         <v>34</v>
       </c>
       <c r="Y18" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z18" s="3" t="s">
         <v>39</v>
@@ -2578,7 +2578,7 @@
         <v>6</v>
       </c>
       <c r="AC18" s="30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AD18" t="s">
         <v>36</v>
@@ -2589,7 +2589,7 @@
     </row>
     <row r="19" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>31</v>
@@ -2662,7 +2662,7 @@
         <v>34</v>
       </c>
       <c r="Y19" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z19" s="3" t="s">
         <v>39</v>
@@ -2674,7 +2674,7 @@
         <v>5</v>
       </c>
       <c r="AC19" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD19" t="s">
         <v>36</v>
@@ -2685,7 +2685,7 @@
     </row>
     <row r="20" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>31</v>
@@ -2758,10 +2758,10 @@
         <v>34</v>
       </c>
       <c r="Y20" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z20" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AA20" s="23" t="s">
         <v>38</v>
@@ -2770,7 +2770,7 @@
         <v>8</v>
       </c>
       <c r="AC20" s="30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AD20" t="s">
         <v>36</v>
@@ -2781,7 +2781,7 @@
     </row>
     <row r="21" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>31</v>
@@ -2854,10 +2854,10 @@
         <v>34</v>
       </c>
       <c r="Y21" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z21" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AA21" s="23" t="s">
         <v>20</v>
@@ -2866,7 +2866,7 @@
         <v>7</v>
       </c>
       <c r="AC21" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD21" t="s">
         <v>36</v>
@@ -2877,7 +2877,7 @@
     </row>
     <row r="22" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>31</v>
@@ -2950,10 +2950,10 @@
         <v>34</v>
       </c>
       <c r="Y22" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z22" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AA22" s="23" t="s">
         <v>38</v>
@@ -2962,7 +2962,7 @@
         <v>10</v>
       </c>
       <c r="AC22" s="30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AD22" t="s">
         <v>36</v>
@@ -2973,7 +2973,7 @@
     </row>
     <row r="23" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>31</v>
@@ -3046,10 +3046,10 @@
         <v>34</v>
       </c>
       <c r="Y23" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z23" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AA23" s="23" t="s">
         <v>20</v>
@@ -3058,7 +3058,7 @@
         <v>9</v>
       </c>
       <c r="AC23" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD23" t="s">
         <v>36</v>
@@ -3069,7 +3069,7 @@
     </row>
     <row r="24" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>31</v>
@@ -3142,10 +3142,10 @@
         <v>34</v>
       </c>
       <c r="Y24" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z24" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AA24" s="23" t="s">
         <v>38</v>
@@ -3154,7 +3154,7 @@
         <v>12</v>
       </c>
       <c r="AC24" s="30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AD24" t="s">
         <v>36</v>
@@ -3165,7 +3165,7 @@
     </row>
     <row r="25" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>31</v>
@@ -3238,10 +3238,10 @@
         <v>34</v>
       </c>
       <c r="Y25" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z25" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AA25" s="23" t="s">
         <v>20</v>
@@ -3250,7 +3250,7 @@
         <v>11</v>
       </c>
       <c r="AC25" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD25" t="s">
         <v>36</v>
@@ -3261,7 +3261,7 @@
     </row>
     <row r="26" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>31</v>
@@ -3334,10 +3334,10 @@
         <v>34</v>
       </c>
       <c r="Y26" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z26" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AA26" s="23" t="s">
         <v>38</v>
@@ -3346,7 +3346,7 @@
         <v>14</v>
       </c>
       <c r="AC26" s="30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AD26" t="s">
         <v>36</v>
@@ -3357,7 +3357,7 @@
     </row>
     <row r="27" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>31</v>
@@ -3430,10 +3430,10 @@
         <v>34</v>
       </c>
       <c r="Y27" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z27" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AA27" s="23" t="s">
         <v>20</v>
@@ -3442,7 +3442,7 @@
         <v>13</v>
       </c>
       <c r="AC27" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD27" t="s">
         <v>36</v>
@@ -3453,7 +3453,7 @@
     </row>
     <row r="28" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>31</v>
@@ -3526,7 +3526,7 @@
         <v>34</v>
       </c>
       <c r="Y28" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z28" s="3" t="s">
         <v>37</v>
@@ -3538,7 +3538,7 @@
         <v>18</v>
       </c>
       <c r="AC28" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD28" t="s">
         <v>36</v>
@@ -3549,7 +3549,7 @@
     </row>
     <row r="29" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>31</v>
@@ -3622,7 +3622,7 @@
         <v>34</v>
       </c>
       <c r="Y29" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z29" s="3" t="s">
         <v>37</v>
@@ -3634,7 +3634,7 @@
         <v>17</v>
       </c>
       <c r="AC29" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD29" t="s">
         <v>36</v>
@@ -3645,7 +3645,7 @@
     </row>
     <row r="30" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>31</v>
@@ -3718,7 +3718,7 @@
         <v>34</v>
       </c>
       <c r="Y30" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z30" s="3" t="s">
         <v>38</v>
@@ -3730,7 +3730,7 @@
         <v>16</v>
       </c>
       <c r="AC30" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD30" t="s">
         <v>36</v>
@@ -3741,7 +3741,7 @@
     </row>
     <row r="31" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>31</v>
@@ -3814,7 +3814,7 @@
         <v>34</v>
       </c>
       <c r="Y31" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z31" s="3" t="s">
         <v>38</v>
@@ -3826,7 +3826,7 @@
         <v>15</v>
       </c>
       <c r="AC31" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD31" t="s">
         <v>36</v>
@@ -3837,7 +3837,7 @@
     </row>
     <row r="32" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>31</v>
@@ -3910,10 +3910,10 @@
         <v>34</v>
       </c>
       <c r="Y32" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z32" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AA32" s="23" t="s">
         <v>38</v>
@@ -3922,7 +3922,7 @@
         <v>20</v>
       </c>
       <c r="AC32" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD32" t="s">
         <v>36</v>
@@ -3933,7 +3933,7 @@
     </row>
     <row r="33" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>31</v>
@@ -4006,10 +4006,10 @@
         <v>34</v>
       </c>
       <c r="Y33" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z33" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AA33" s="23" t="s">
         <v>20</v>
@@ -4018,7 +4018,7 @@
         <v>19</v>
       </c>
       <c r="AC33" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD33" t="s">
         <v>36</v>
@@ -4029,7 +4029,7 @@
     </row>
     <row r="34" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B34" s="18" t="s">
         <v>31</v>
@@ -4105,7 +4105,7 @@
         <v>38</v>
       </c>
       <c r="Z34" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AA34" s="25" t="s">
         <v>20</v>
@@ -4114,18 +4114,18 @@
         <v>26</v>
       </c>
       <c r="AC34" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD34" t="s">
         <v>36</v>
       </c>
       <c r="AE34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B35" s="18" t="s">
         <v>31</v>
@@ -4201,7 +4201,7 @@
         <v>37</v>
       </c>
       <c r="Z35" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AA35" s="25" t="s">
         <v>20</v>
@@ -4210,18 +4210,18 @@
         <v>27</v>
       </c>
       <c r="AC35" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD35" t="s">
         <v>36</v>
       </c>
       <c r="AE35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>31</v>
@@ -4297,7 +4297,7 @@
         <v>38</v>
       </c>
       <c r="Z36" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AA36" s="23" t="s">
         <v>20</v>
@@ -4306,18 +4306,18 @@
         <v>28</v>
       </c>
       <c r="AC36" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD36" t="s">
         <v>36</v>
       </c>
       <c r="AE36" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>31</v>
@@ -4393,7 +4393,7 @@
         <v>37</v>
       </c>
       <c r="Z37" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AA37" s="23" t="s">
         <v>20</v>
@@ -4402,18 +4402,18 @@
         <v>29</v>
       </c>
       <c r="AC37" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD37" t="s">
         <v>36</v>
       </c>
       <c r="AE37" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>31</v>
@@ -4489,7 +4489,7 @@
         <v>39</v>
       </c>
       <c r="Z38" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AA38" s="23" t="s">
         <v>20</v>
@@ -4498,18 +4498,18 @@
         <v>30</v>
       </c>
       <c r="AC38" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD38" t="s">
         <v>36</v>
       </c>
       <c r="AE38" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B39" s="18" t="s">
         <v>31</v>
@@ -4582,10 +4582,10 @@
         <v>34</v>
       </c>
       <c r="Y39" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Z39" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AA39" s="23" t="s">
         <v>20</v>
@@ -4594,18 +4594,18 @@
         <v>31</v>
       </c>
       <c r="AC39" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD39" t="s">
         <v>36</v>
       </c>
       <c r="AE39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>31</v>
@@ -4678,10 +4678,10 @@
         <v>34</v>
       </c>
       <c r="Y40" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Z40" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AA40" s="23" t="s">
         <v>38</v>
@@ -4690,18 +4690,18 @@
         <v>32</v>
       </c>
       <c r="AC40" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD40" t="s">
         <v>36</v>
       </c>
       <c r="AE40" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B41" s="18" t="s">
         <v>31</v>
@@ -4774,10 +4774,10 @@
         <v>34</v>
       </c>
       <c r="Y41" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Z41" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AA41" s="23" t="s">
         <v>37</v>
@@ -4786,18 +4786,18 @@
         <v>33</v>
       </c>
       <c r="AC41" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD41" t="s">
         <v>36</v>
       </c>
       <c r="AE41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B42" s="18" t="s">
         <v>31</v>
@@ -4870,30 +4870,30 @@
         <v>34</v>
       </c>
       <c r="Y42" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Z42" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AA42" s="23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AB42" s="3">
         <v>34</v>
       </c>
       <c r="AC42" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD42" t="s">
         <v>36</v>
       </c>
       <c r="AE42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B43" s="18" t="s">
         <v>31</v>
@@ -4966,10 +4966,10 @@
         <v>34</v>
       </c>
       <c r="Y43" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Z43" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AA43" s="23" t="s">
         <v>39</v>
@@ -4978,18 +4978,18 @@
         <v>35</v>
       </c>
       <c r="AC43" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD43" t="s">
         <v>36</v>
       </c>
       <c r="AE43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B44" s="18" t="s">
         <v>31</v>
@@ -5062,10 +5062,10 @@
         <v>34</v>
       </c>
       <c r="Y44" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Z44" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AA44" s="23" t="s">
         <v>20</v>
@@ -5074,18 +5074,18 @@
         <v>36</v>
       </c>
       <c r="AC44" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD44" t="s">
         <v>36</v>
       </c>
       <c r="AE44" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B45" s="18" t="s">
         <v>31</v>
@@ -5158,10 +5158,10 @@
         <v>34</v>
       </c>
       <c r="Y45" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Z45" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AA45" s="23" t="s">
         <v>20</v>
@@ -5170,18 +5170,18 @@
         <v>21</v>
       </c>
       <c r="AC45" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD45" t="s">
         <v>36</v>
       </c>
       <c r="AE45" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B46" s="18" t="s">
         <v>31</v>
@@ -5254,10 +5254,10 @@
         <v>34</v>
       </c>
       <c r="Y46" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Z46" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AA46" s="23" t="s">
         <v>20</v>
@@ -5266,18 +5266,18 @@
         <v>22</v>
       </c>
       <c r="AC46" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD46" t="s">
         <v>36</v>
       </c>
       <c r="AE46" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B47" s="18" t="s">
         <v>31</v>
@@ -5350,10 +5350,10 @@
         <v>34</v>
       </c>
       <c r="Y47" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Z47" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AA47" s="23" t="s">
         <v>20</v>
@@ -5362,18 +5362,18 @@
         <v>23</v>
       </c>
       <c r="AC47" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD47" t="s">
         <v>36</v>
       </c>
       <c r="AE47" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B48" s="18" t="s">
         <v>31</v>
@@ -5446,10 +5446,10 @@
         <v>34</v>
       </c>
       <c r="Y48" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Z48" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="AA48" s="23" t="s">
         <v>20</v>
@@ -5458,18 +5458,18 @@
         <v>24</v>
       </c>
       <c r="AC48" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD48" t="s">
         <v>36</v>
       </c>
       <c r="AE48" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B49" s="18" t="s">
         <v>31</v>
@@ -5542,25 +5542,25 @@
         <v>34</v>
       </c>
       <c r="Y49" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Z49" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AA49" s="23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AB49" s="3">
         <v>25</v>
       </c>
       <c r="AC49" s="30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AD49" t="s">
         <v>36</v>
       </c>
       <c r="AE49" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>